<commit_message>
fix: correct fields format because test fail
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_35fd\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D3E04B0-C55D-41BE-8702-CFFC46A8262B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47E9B1C4-82BA-4012-997D-165F3E5CB183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -151,6 +151,9 @@
     <t>Jeune</t>
   </si>
   <si>
+    <t>182.12</t>
+  </si>
+  <si>
     <t>Argilo-sableux</t>
   </si>
   <si>
@@ -206,6 +209,12 @@
   </si>
   <si>
     <t>Adulte</t>
+  </si>
+  <si>
+    <t>229.10</t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
   <si>
     <t>Argileux</t>
@@ -290,6 +299,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -767,9 +779,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1127,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1238,7 +1251,7 @@
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>43385</v>
       </c>
       <c r="E2" t="s">
@@ -1265,7 +1278,7 @@
       <c r="M2">
         <v>259001</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="2">
         <v>43232</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -1277,42 +1290,41 @@
       <c r="Q2">
         <v>58</v>
       </c>
-      <c r="R2">
-        <f>Q2*3.14</f>
-        <v>182.12</v>
+      <c r="R2" t="s">
+        <v>39</v>
       </c>
       <c r="S2">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Y2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Z2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AB2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AD2">
         <v>3</v>
@@ -1323,28 +1335,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="1">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2">
         <v>44306</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J3">
         <v>13055</v>
@@ -1353,16 +1365,16 @@
         <v>13001</v>
       </c>
       <c r="L3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="1">
+        <v>57</v>
+      </c>
+      <c r="N3" s="2">
         <v>35905</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P3">
         <v>235</v>
@@ -1370,39 +1382,38 @@
       <c r="Q3">
         <v>73</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3" si="0">Q3*3.14</f>
-        <v>229.22</v>
-      </c>
-      <c r="S3">
-        <v>1.5</v>
+      <c r="R3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" t="s">
+        <v>60</v>
       </c>
       <c r="T3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="U3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="V3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="X3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Y3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Z3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AA3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AB3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -1410,25 +1421,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="1">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2">
         <v>35855</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J4">
         <v>13055</v>
@@ -1437,31 +1448,31 @@
         <v>13002</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="1">
+        <v>73</v>
+      </c>
+      <c r="N4" s="2">
         <v>32933</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="X4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Y4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AB4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AD4">
         <v>2</v>
       </c>
       <c r="AE4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -1469,22 +1480,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J5">
         <v>13055</v>
@@ -1493,28 +1504,28 @@
         <v>13013</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="O5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="T5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="U5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="V5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="W5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="X5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>